<commit_message>
Aug 21, 2015 Update
</commit_message>
<xml_diff>
--- a/Coding Reference.xlsx
+++ b/Coding Reference.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="587" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="416">
   <si>
     <t>Refer to column</t>
   </si>
@@ -1219,6 +1219,87 @@
   </si>
   <si>
     <t>part of 'scales' package</t>
+  </si>
+  <si>
+    <t>df[~df['col'].isin(['ye','boi'])]</t>
+  </si>
+  <si>
+    <t>#3 is NOT in</t>
+  </si>
+  <si>
+    <t>Add. Args: index = False</t>
+  </si>
+  <si>
+    <t>String Character Length</t>
+  </si>
+  <si>
+    <t>transform(df, Length=nchar(as.character(A)))</t>
+  </si>
+  <si>
+    <t>Approximate Match</t>
+  </si>
+  <si>
+    <t>agrep('string',df$A)</t>
+  </si>
+  <si>
+    <t>Returns location</t>
+  </si>
+  <si>
+    <t>Count Uniques within Dimension</t>
+  </si>
+  <si>
+    <t>df.groupby('A').CountItem.nunique()</t>
+  </si>
+  <si>
+    <t>Conver to Pandas DF</t>
+  </si>
+  <si>
+    <t>Count IF</t>
+  </si>
+  <si>
+    <t>sum(df$a=='ye',na.rm=T)</t>
+  </si>
+  <si>
+    <t>Categorize Based on Value</t>
+  </si>
+  <si>
+    <t>df['b'] = np.where(df['a'] &gt; 5,'high','low')</t>
+  </si>
+  <si>
+    <t>Match items on list</t>
+  </si>
+  <si>
+    <t>match(df$a,matchtable)</t>
+  </si>
+  <si>
+    <t>nomatch = 0</t>
+  </si>
+  <si>
+    <t>df$a[which(df$a&gt;0)]&lt;-1</t>
+  </si>
+  <si>
+    <t>Change values conditionally</t>
+  </si>
+  <si>
+    <t>Match (Intersection)</t>
+  </si>
+  <si>
+    <t>set(df1) &amp; set(df2)</t>
+  </si>
+  <si>
+    <t>Add. Args: regex = True (for part of a string)</t>
+  </si>
+  <si>
+    <t>Keep Columns</t>
+  </si>
+  <si>
+    <t>df[['a','b']]</t>
+  </si>
+  <si>
+    <t>Keep first occurrence</t>
+  </si>
+  <si>
+    <t>df.groupby('a').first()</t>
   </si>
 </sst>
 </file>
@@ -1554,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1789,6 +1870,12 @@
       <c r="D14" t="s">
         <v>47</v>
       </c>
+      <c r="E14" t="s">
+        <v>389</v>
+      </c>
+      <c r="F14" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1921,13 +2008,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>267</v>
       </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
       <c r="C24" t="s">
         <v>322</v>
+      </c>
+      <c r="F24" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2282,6 +2372,9 @@
       <c r="D49" t="s">
         <v>246</v>
       </c>
+      <c r="F49" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -2543,6 +2636,51 @@
       </c>
       <c r="C69" t="s">
         <v>323</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>397</v>
+      </c>
+      <c r="C70" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>402</v>
+      </c>
+      <c r="C72" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>409</v>
+      </c>
+      <c r="C73" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>412</v>
+      </c>
+      <c r="C74" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>414</v>
+      </c>
+      <c r="C75" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -2553,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3413,6 +3551,55 @@
       </c>
       <c r="F67" t="s">
         <v>388</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>392</v>
+      </c>
+      <c r="C68" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>394</v>
+      </c>
+      <c r="C69" t="s">
+        <v>395</v>
+      </c>
+      <c r="F69" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>400</v>
+      </c>
+      <c r="C70" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>404</v>
+      </c>
+      <c r="C71" t="s">
+        <v>405</v>
+      </c>
+      <c r="F71" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>408</v>
+      </c>
+      <c r="C72" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>